<commit_message>
Algunos cambios para poder hacer ejecutable
</commit_message>
<xml_diff>
--- a/Fer_actualizar.xlsx
+++ b/Fer_actualizar.xlsx
@@ -612,7 +612,7 @@
         <v/>
       </c>
       <c r="I2" s="7" t="n">
-        <v>471.7719518</v>
+        <v>525.11</v>
       </c>
       <c r="J2" s="8" t="n"/>
       <c r="K2" s="13">
@@ -654,7 +654,7 @@
         <v/>
       </c>
       <c r="I3" s="7" t="n">
-        <v>159.4345005</v>
+        <v>177.46</v>
       </c>
       <c r="J3" s="8" t="n"/>
       <c r="K3" s="13">
@@ -696,7 +696,7 @@
         <v/>
       </c>
       <c r="I4" s="7" t="n">
-        <v>177.492843</v>
+        <v>197.56</v>
       </c>
       <c r="J4" s="8" t="n"/>
       <c r="K4" s="13">
@@ -738,7 +738,7 @@
         <v/>
       </c>
       <c r="I5" s="7" t="n">
-        <v>218.5957868</v>
+        <v>243.31</v>
       </c>
       <c r="J5" s="8" t="n"/>
       <c r="K5" s="13">
@@ -780,7 +780,7 @@
         <v/>
       </c>
       <c r="I6" s="7" t="n">
-        <v>223.9773525</v>
+        <v>249.3</v>
       </c>
       <c r="J6" s="8" t="n"/>
       <c r="K6" s="13">
@@ -822,7 +822,7 @@
         <v/>
       </c>
       <c r="I7" s="7" t="n">
-        <v>229.745241</v>
+        <v>255.72</v>
       </c>
       <c r="J7" s="8" t="n"/>
       <c r="K7" s="13">
@@ -864,7 +864,7 @@
         <v/>
       </c>
       <c r="I8" s="7" t="n">
-        <v>247.4172608</v>
+        <v>275.39</v>
       </c>
       <c r="J8" s="8" t="n"/>
       <c r="K8" s="13">
@@ -906,7 +906,7 @@
         <v/>
       </c>
       <c r="I9" s="7" t="n">
-        <v>248.9535675</v>
+        <v>277.1</v>
       </c>
       <c r="J9" s="8" t="n"/>
       <c r="K9" s="13">
@@ -948,7 +948,7 @@
         <v/>
       </c>
       <c r="I10" s="7" t="n">
-        <v>256.6351013</v>
+        <v>285.65</v>
       </c>
       <c r="J10" s="8" t="n"/>
       <c r="K10" s="13">
@@ -990,7 +990,7 @@
         <v/>
       </c>
       <c r="I11" s="7" t="n">
-        <v>263.166651</v>
+        <v>292.92</v>
       </c>
       <c r="J11" s="8" t="n"/>
       <c r="K11" s="13">
@@ -1032,7 +1032,7 @@
         <v/>
       </c>
       <c r="I12" s="7" t="n">
-        <v>270.0845235</v>
+        <v>300.62</v>
       </c>
       <c r="J12" s="8" t="n"/>
       <c r="K12" s="13">
@@ -1074,7 +1074,7 @@
         <v/>
       </c>
       <c r="I13" s="7" t="n">
-        <v>276.2297505</v>
+        <v>307.46</v>
       </c>
       <c r="J13" s="8" t="n"/>
       <c r="K13" s="13">
@@ -1116,7 +1116,7 @@
         <v/>
       </c>
       <c r="I14" s="7" t="n">
-        <v>281.9886548</v>
+        <v>313.87</v>
       </c>
       <c r="J14" s="8" t="n"/>
       <c r="K14" s="13">
@@ -1158,7 +1158,7 @@
         <v/>
       </c>
       <c r="I15" s="7" t="n">
-        <v>281.9886548</v>
+        <v>313.87</v>
       </c>
       <c r="J15" s="8" t="n"/>
       <c r="K15" s="13">

</xml_diff>